<commit_message>
Add packages and modify sdk
</commit_message>
<xml_diff>
--- a/Project_Files/Pending Tasks.xlsx
+++ b/Project_Files/Pending Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\task_management_system\Project_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Freelance_Projects\Task_Management_System\Project_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA41A7F5-8349-4D80-B1A7-FF1653965E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03ACC68-C782-46C2-96E0-06D6732D8EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" xr2:uid="{5319EC15-A4E2-4DCC-9627-9642AE7DFA29}"/>
+    <workbookView xWindow="13005" yWindow="11340" windowWidth="16440" windowHeight="9075" xr2:uid="{5319EC15-A4E2-4DCC-9627-9642AE7DFA29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Pending Tasks</t>
   </si>
@@ -82,13 +82,25 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Logout for employee</t>
-  </si>
-  <si>
     <t>tab to navigate in dashboard</t>
   </si>
   <si>
     <t>select employee from ddl</t>
+  </si>
+  <si>
+    <t>Manager Task Delete</t>
+  </si>
+  <si>
+    <t>Filter Tasks</t>
+  </si>
+  <si>
+    <t>Filter Employees in tasks</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Fix Name in dahsboard</t>
   </si>
 </sst>
 </file>
@@ -111,12 +123,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,16 +146,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -155,8 +176,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9978120-486C-43C8-8BE3-482E9E025417}" name="Table1" displayName="Table1" ref="A1:B13" totalsRowShown="0">
-  <autoFilter ref="A1:B13" xr:uid="{B9978120-486C-43C8-8BE3-482E9E025417}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9978120-486C-43C8-8BE3-482E9E025417}" name="Table1" displayName="Table1" ref="A1:B14" totalsRowShown="0">
+  <autoFilter ref="A1:B14" xr:uid="{B9978120-486C-43C8-8BE3-482E9E025417}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
+    <sortCondition ref="B1:B14"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D65EF770-7BB6-4641-99F2-D9ABA8F8190A}" name="Pending Tasks"/>
     <tableColumn id="2" xr3:uid="{E154CA15-5E3D-4168-BC2B-0D1E7DAB8F73}" name="% Percentage"/>
@@ -462,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3F41B5-E607-432D-A6BC-A65B06391757}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,23 +508,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -508,7 +532,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -516,52 +540,78 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2" cm="1">
-        <f t="array" ref="B13">SUM(B2:B12 / COUNT(B2:B12))</f>
-        <v>0.22500000000000001</v>
+      <c r="B15" s="3" cm="1">
+        <f t="array" ref="B15">SUM(B2:B14 / COUNT(B2:B14))</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>